<commit_message>
update on the community health area
</commit_message>
<xml_diff>
--- a/forms/contact/community_health_area-create.xlsx
+++ b/forms/contact/community_health_area-create.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7770" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -850,10 +850,10 @@
     <t>roles</t>
   </si>
   <si>
-    <t>chw</t>
-  </si>
-  <si>
-    <t>CHW</t>
+    <t>chp</t>
+  </si>
+  <si>
+    <t>CHP</t>
   </si>
   <si>
     <t>सामुदायिक स्वास्थ्य कर्मी</t>
@@ -871,10 +871,10 @@
     <t>ASC</t>
   </si>
   <si>
-    <t>chw_supervisor</t>
-  </si>
-  <si>
-    <t>CHW Supervisor</t>
+    <t>chp_supervisor</t>
+  </si>
+  <si>
+    <t>CHP Supervisor</t>
   </si>
   <si>
     <t>सामुदायिक स्वास्थ्य कर्मी के मैनेजर</t>
@@ -1161,10 +1161,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1207,30 +1207,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1244,32 +1222,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1284,8 +1246,61 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1305,36 +1320,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -1344,15 +1329,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1427,19 +1427,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1451,25 +1451,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1487,19 +1475,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1517,49 +1571,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1571,43 +1607,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1618,6 +1618,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1651,21 +1684,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1673,33 +1691,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1718,141 +1709,150 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2121,11 +2121,11 @@
   <dimension ref="A1:AR70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A44" sqref="A44"/>
+      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.437037037037" defaultRowHeight="15"/>
@@ -6176,7 +6176,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A21" sqref="$A21:$XFD25"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.437037037037" defaultRowHeight="15"/>
@@ -6942,7 +6942,7 @@
       </c>
       <c r="C2" s="2" t="str">
         <f ca="1">TEXT(NOW(),"yyyy-mm-dd_HH-MM")</f>
-        <v>2024-04-17 12-10</v>
+        <v>2024-04-30 10-21</v>
       </c>
       <c r="D2" t="s">
         <v>376</v>

</xml_diff>